<commit_message>
update duerer data: media urls and fix media id links
</commit_message>
<xml_diff>
--- a/public/data/data-duerer-macro.xlsx
+++ b/public/data/data-duerer-macro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5867A7EB-7FB0-4DA6-8C91-6F1DA14377CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B363D1-6217-4BEB-8442-BE7C06F1DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="539">
   <si>
     <t>id</t>
   </si>
@@ -1243,9 +1243,6 @@
     <t>m-023</t>
   </si>
   <si>
-    <t>https://www.bildindex.de/media/large/mi/03/97/6a/mi03976a05.jpg?Expires=1677759882&amp;Signature=hWeVgz5cjlYCBB2LCiBgpEX8KcG3RfTFq0uPL84nDEqrdHhy5ubRwrJVjKuEWzf92X13ypwWFMGToksoUmCw2HPJSF~1JI8zBmob43tSWRXG7P0H5U3DKehqf2tfXUma7o~ZU42ct2Rf9FcwuOsC6EEw2QvAlzU7pO6W7wfrA18_&amp;Key-Pair-Id=APKAJGHHKKX2FHRP63AQ</t>
-  </si>
-  <si>
     <t>https://www.bildindex.de/document/obj00030696?medium=mi03976a05&amp;part=1</t>
   </si>
   <si>
@@ -1345,9 +1342,6 @@
     <t>Two Castles</t>
   </si>
   <si>
-    <t>http://images.zeno.org/Kunstwerke/I/big/2540011a.jpg</t>
-  </si>
-  <si>
     <t>https://sammlung.staedelmuseum.de/en/work/marx-ulstat-the-beautiful-young-woman-of-antwerp</t>
   </si>
   <si>
@@ -1495,9 +1489,6 @@
     <t>https://commons.wikimedia.org/wiki/File:Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/e/e6/Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif</t>
-  </si>
-  <si>
     <t>m-038</t>
   </si>
   <si>
@@ -1649,6 +1640,30 @@
   </si>
   <si>
     <t>is gravesite</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1DI1Ih544jL7rxyUxA_urkV1GCl2LMEN_</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1g0sQAaHO8xrO0id89bB5WEoTsmN3C4bw</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1MwHz0Y-xqQ4XhFbmHQF9m4Lh9uaOPLvW</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1kJEGUnYN_fdjPG26fQpJVWzIfQqmXIqt</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1ofODJ9GwqtRlt_Cr4eDdi_IeEAs72j5b</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1c_AeKhXQrgmen6fqNzQ7C41dHJtmICSK</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=download&amp;id=1PU60_TqWqGJoRRiKm8-sOteLeKhF7vVq</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e6/Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif/lossy-page1-775px-Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif.jpg</t>
   </si>
 </sst>
 </file>
@@ -1794,8 +1809,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2114,7 +2129,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2344,7 +2359,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>208</v>
@@ -2364,7 +2379,7 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2437,7 +2452,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>180</v>
@@ -2454,10 +2469,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>180</v>
@@ -2477,7 +2492,7 @@
         <v>156</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>186</v>
@@ -2497,7 +2512,7 @@
         <v>156</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>186</v>
@@ -2514,10 +2529,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>186</v>
@@ -2535,7 +2550,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>181</v>
@@ -2554,10 +2569,10 @@
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>215</v>
@@ -2603,10 +2618,10 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H12" t="s">
         <v>180</v>
@@ -4585,8 +4600,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4594,7 +4609,7 @@
     <col min="1" max="1" width="8.9375" style="3"/>
     <col min="2" max="2" width="38.29296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="64.703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="57.9375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="57.9375" customWidth="1"/>
     <col min="5" max="5" width="11.52734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.76171875" style="3" customWidth="1"/>
     <col min="7" max="16384" width="8.9375" style="3"/>
@@ -4654,7 +4669,7 @@
         <v>344</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -4667,7 +4682,9 @@
       <c r="C4" s="24" t="s">
         <v>364</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="27" t="s">
+        <v>531</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>344</v>
       </c>
@@ -4714,7 +4731,7 @@
         <v>380</v>
       </c>
       <c r="B7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>378</v>
@@ -4726,7 +4743,7 @@
         <v>344</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -4737,10 +4754,10 @@
         <v>223</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>399</v>
-      </c>
-      <c r="D8" s="24" t="s">
         <v>398</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>532</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>344</v>
@@ -4754,10 +4771,10 @@
         <v>224</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>404</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>405</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>344</v>
@@ -4771,10 +4788,10 @@
         <v>225</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>344</v>
@@ -4788,16 +4805,16 @@
         <v>226</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>408</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>409</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -4805,19 +4822,19 @@
         <v>386</v>
       </c>
       <c r="B12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="D12" t="s">
         <v>410</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>411</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -4828,16 +4845,16 @@
         <v>220</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>413</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>414</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -4848,16 +4865,16 @@
         <v>227</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -4868,9 +4885,11 @@
         <v>228</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>418</v>
-      </c>
-      <c r="D15" s="26"/>
+        <v>417</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>533</v>
+      </c>
       <c r="E15" s="3" t="s">
         <v>344</v>
       </c>
@@ -4883,10 +4902,10 @@
         <v>229</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>344</v>
@@ -4900,10 +4919,10 @@
         <v>230</v>
       </c>
       <c r="C17" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="D17" t="s">
         <v>421</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>422</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>344</v>
@@ -4917,16 +4936,16 @@
         <v>231</v>
       </c>
       <c r="C18" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>423</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>424</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -4937,10 +4956,10 @@
         <v>232</v>
       </c>
       <c r="C19" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>425</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>426</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>344</v>
@@ -4954,10 +4973,10 @@
         <v>233</v>
       </c>
       <c r="C20" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="D20" t="s">
         <v>427</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>428</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>344</v>
@@ -4968,19 +4987,19 @@
         <v>394</v>
       </c>
       <c r="B21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>430</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>432</v>
+        <v>429</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>534</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -4988,12 +5007,14 @@
         <v>395</v>
       </c>
       <c r="B22" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>433</v>
-      </c>
-      <c r="D22" s="26"/>
+        <v>431</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>535</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>344</v>
       </c>
@@ -5006,10 +5027,10 @@
         <v>234</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
+      </c>
+      <c r="D23" t="s">
+        <v>442</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>344</v>
@@ -5023,10 +5044,10 @@
         <v>235</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
+      </c>
+      <c r="D24" t="s">
+        <v>443</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>344</v>
@@ -5034,16 +5055,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B25" t="s">
         <v>236</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>446</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
+      </c>
+      <c r="D25" t="s">
+        <v>445</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>344</v>
@@ -5051,16 +5072,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B26" t="s">
         <v>237</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>448</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
+      </c>
+      <c r="D26" t="s">
+        <v>447</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>344</v>
@@ -5068,13 +5089,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B27" t="s">
         <v>238</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>450</v>
+        <v>448</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>536</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>344</v>
@@ -5082,16 +5106,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B28" t="s">
         <v>239</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>344</v>
@@ -5099,16 +5123,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B29" t="s">
         <v>240</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>453</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
+      </c>
+      <c r="D29" t="s">
+        <v>452</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>344</v>
@@ -5116,36 +5140,36 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B30" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C30" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>455</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>457</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B31" t="s">
         <v>241</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>459</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>458</v>
+        <v>457</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>456</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>344</v>
@@ -5153,53 +5177,56 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B32" t="s">
         <v>242</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>460</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
+      </c>
+      <c r="D32" t="s">
+        <v>459</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B33" t="s">
         <v>243</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
+      </c>
+      <c r="D33" t="s">
+        <v>461</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B34" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>537</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>344</v>
@@ -5207,36 +5234,36 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>470</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
+      </c>
+      <c r="D36" t="s">
+        <v>469</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>344</v>
@@ -5244,16 +5271,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C37" s="24" t="s">
         <v>473</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>475</v>
-      </c>
       <c r="D37" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>344</v>
@@ -5261,36 +5288,36 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>477</v>
+      </c>
+      <c r="D38" s="26" t="s">
         <v>478</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>479</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>480</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>481</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>538</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>344</v>
@@ -5298,214 +5325,220 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>505</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
+      </c>
+      <c r="D43" t="s">
+        <v>503</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{6555C001-AF61-499A-ABE7-287E901E3F73}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{3A277AAE-8FCE-499A-AE78-309DEB57D14E}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{FF537007-C8B6-422B-B764-A977081C356D}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{01803DF9-95A9-4673-B3CF-0AFDC51738A6}"/>
-    <hyperlink ref="D5" r:id="rId5" xr:uid="{2035CEB9-3894-4D0E-A800-0EDCBF47DCB0}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{0A79A952-20B9-42A0-96C2-1DF0D3009FCE}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{C448F71C-0442-4884-8E94-74AB850D546C}"/>
-    <hyperlink ref="D6" r:id="rId8" xr:uid="{7D5EB142-335B-4476-B272-FD9F53933C39}"/>
-    <hyperlink ref="C6" r:id="rId9" xr:uid="{CCDBF689-403E-43A8-BED9-3E755171E066}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{64183D9C-D3CF-4202-B5C3-18F54B30105D}"/>
-    <hyperlink ref="D8" r:id="rId11" display="https://www.bildindex.de/media/large/mi/03/97/6a/mi03976a05.jpg?Expires=1677759882&amp;Signature=hWeVgz5cjlYCBB2LCiBgpEX8KcG3RfTFq0uPL84nDEqrdHhy5ubRwrJVjKuEWzf92X13ypwWFMGToksoUmCw2HPJSF~1JI8zBmob43tSWRXG7P0H5U3DKehqf2tfXUma7o~ZU42ct2Rf9FcwuOsC6EEw2QvAlzU7pO6W7wfrA18_&amp;Key-Pair-Id=APKAJGHHKKX2FHRP63AQ" xr:uid="{2BDCDC4C-CAC4-44B7-B28C-83BD8753952C}"/>
-    <hyperlink ref="C8" r:id="rId12" xr:uid="{63355708-FBD7-4D22-AECF-34AD1D7C138F}"/>
-    <hyperlink ref="C9" r:id="rId13" xr:uid="{480D5B27-8454-41B3-A50B-4ACFFDAE4026}"/>
-    <hyperlink ref="D9" r:id="rId14" xr:uid="{1E9B9CA0-D6F1-4AE0-AE43-7776F5BD6EF1}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{EA214F1E-4812-477F-90AE-31C9F30296F1}"/>
-    <hyperlink ref="C10" r:id="rId16" xr:uid="{9FE6D3D1-53E9-489A-AB96-5EC7DADDD591}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{B87A9B74-3BD6-4ED9-98AB-34EDAE07337F}"/>
-    <hyperlink ref="C12" r:id="rId18" xr:uid="{5D03CC0B-DEE3-4FDE-9306-CE5E26709C32}"/>
-    <hyperlink ref="C13" r:id="rId19" xr:uid="{FFAAC713-605F-4948-894C-B32F62D6C8E4}"/>
-    <hyperlink ref="D13" r:id="rId20" xr:uid="{A0893C3E-1C28-467D-9AFC-E8EE4AB9FB89}"/>
-    <hyperlink ref="D14" r:id="rId21" xr:uid="{3F64321A-2515-493E-917E-72B791B9408D}"/>
-    <hyperlink ref="C14" r:id="rId22" xr:uid="{0332E7E1-BC6A-47EA-89D6-97A7068AB01F}"/>
-    <hyperlink ref="C15" r:id="rId23" xr:uid="{6EC68279-7666-4082-ADEA-A2C7658064D2}"/>
-    <hyperlink ref="D16" r:id="rId24" xr:uid="{517CD509-8487-4373-A454-B2B9E47FF545}"/>
-    <hyperlink ref="C16" r:id="rId25" xr:uid="{29844E65-FF0E-4D48-82B8-096506F811E6}"/>
-    <hyperlink ref="C17" r:id="rId26" xr:uid="{28A376E3-CC6D-491B-96A1-EB17AA4EFB22}"/>
-    <hyperlink ref="C18" r:id="rId27" xr:uid="{412FF679-225E-44C0-8E9F-CFBE4329EBC3}"/>
-    <hyperlink ref="D18" r:id="rId28" xr:uid="{F8DEBD7A-3831-43DB-A095-2BC3CECE35C2}"/>
-    <hyperlink ref="C19" r:id="rId29" xr:uid="{7C9CB129-6FFC-4285-AC98-069E1A3CCCC6}"/>
-    <hyperlink ref="D19" r:id="rId30" xr:uid="{CE60D295-56DA-4DAD-ABF8-FA73AB5B855E}"/>
-    <hyperlink ref="C20" r:id="rId31" xr:uid="{234F6491-E60B-4B87-A632-870076D9CCA7}"/>
-    <hyperlink ref="C21" r:id="rId32" xr:uid="{61D9836A-7C7E-4867-ABF5-33BB8C69892E}"/>
-    <hyperlink ref="D21" r:id="rId33" xr:uid="{ABE00576-9886-4B0A-A870-5D91CF571100}"/>
-    <hyperlink ref="C22" r:id="rId34" xr:uid="{D4605030-C409-4AF3-8259-809032BBDE3E}"/>
-    <hyperlink ref="C25" r:id="rId35" xr:uid="{080340CC-9D67-448D-91B8-CF5E61F24528}"/>
-    <hyperlink ref="C26" r:id="rId36" xr:uid="{2C13BE1F-6959-4279-B9CC-BE2550EA0D05}"/>
-    <hyperlink ref="C27" r:id="rId37" xr:uid="{161A5A2E-4114-4985-9828-82028E172B03}"/>
-    <hyperlink ref="D28" r:id="rId38" xr:uid="{C7E1F470-0BA6-453D-B307-2A7B184F5CBB}"/>
-    <hyperlink ref="C28" r:id="rId39" xr:uid="{11E684AC-C433-4034-B87F-E540C77A524F}"/>
-    <hyperlink ref="C29" r:id="rId40" xr:uid="{6B023398-4DAE-4F93-81D4-CF7601909568}"/>
-    <hyperlink ref="C30" r:id="rId41" xr:uid="{0C9432DA-F217-44DE-B2FF-70283A13F215}"/>
-    <hyperlink ref="D30" r:id="rId42" xr:uid="{5AFC87AF-12FB-4162-8E98-DF8E161DC898}"/>
-    <hyperlink ref="D31" r:id="rId43" xr:uid="{55865B39-4DCB-4D60-B607-52D2D3ADFF82}"/>
-    <hyperlink ref="C31" r:id="rId44" xr:uid="{B70145B5-B167-4A5B-8D5E-B5EBC65F3C2B}"/>
-    <hyperlink ref="C32" r:id="rId45" xr:uid="{ED6D5FE2-EE49-483E-B19B-37602DF833A2}"/>
-    <hyperlink ref="D7" r:id="rId46" xr:uid="{F5CD6900-3559-4D8F-8717-FF92BEE78CF8}"/>
-    <hyperlink ref="C35" r:id="rId47" xr:uid="{DBA5A372-746C-4C4C-815B-81F869194C86}"/>
-    <hyperlink ref="D35" r:id="rId48" xr:uid="{4D09EA8C-4FA5-43D4-83C6-8F98113BD100}"/>
-    <hyperlink ref="C36" r:id="rId49" xr:uid="{FEDE9C89-95F5-405A-B824-83ACDC1592FF}"/>
-    <hyperlink ref="C37" r:id="rId50" xr:uid="{8E39BE0E-9C8D-4504-94B0-4A6D54597337}"/>
-    <hyperlink ref="D37" r:id="rId51" xr:uid="{4F366ACA-E9DC-4D82-A164-F3C23305A963}"/>
-    <hyperlink ref="C38" r:id="rId52" xr:uid="{1ED5BD43-7A12-48C2-BC69-8F0EBCC5B3A0}"/>
-    <hyperlink ref="D38" r:id="rId53" xr:uid="{F2EA09DA-74A9-46C8-AF66-8E4B1AB4C1B9}"/>
-    <hyperlink ref="C39" r:id="rId54" xr:uid="{049280BA-CFC9-44A0-A076-2331B0E40C26}"/>
-    <hyperlink ref="C40" r:id="rId55" xr:uid="{9C52C1E3-7BD1-4B41-A23E-81A351F47D54}"/>
-    <hyperlink ref="D40" r:id="rId56" xr:uid="{EC6045AC-7661-4396-876E-A185378B4D91}"/>
-    <hyperlink ref="C41" r:id="rId57" xr:uid="{D1BD7645-D58F-40F7-978F-383E3AB8995C}"/>
-    <hyperlink ref="D42" r:id="rId58" xr:uid="{6DA96B2C-01E1-4702-8D73-C6CB924302ED}"/>
-    <hyperlink ref="C42" r:id="rId59" xr:uid="{70FE4ABE-035F-4403-A099-051396E69EF1}"/>
-    <hyperlink ref="C43" r:id="rId60" xr:uid="{A6B885F7-852B-4C3F-896A-81B7A4085B52}"/>
-    <hyperlink ref="D45" r:id="rId61" xr:uid="{2AFA1DCA-150C-4E59-B51B-408C4EE4D9F1}"/>
-    <hyperlink ref="C45" r:id="rId62" xr:uid="{7C291294-21B9-4C11-8570-25513F54FB58}"/>
-    <hyperlink ref="C44" r:id="rId63" xr:uid="{CBEA5E2B-AF57-44B8-A639-1B5A04764DA8}"/>
-    <hyperlink ref="D44" r:id="rId64" display="https://books.googleusercontent.com/books/content?req=AKW5QacMsPlzkhSCOohiXYeGljWguMgUQZpwSe9jD-AwX2dY7j4q8PfiYB4m-J-mvsYJpatZ3-Jt4fsCZCAr6gcAHgo8XQBnTUMNt41l5rsg236daxIa9HqNBkAEk1oCCB_F_p0JSetKf7xs-kEVhTq-Qbn_wXgRDnmYyENLKcPb6eOAGx0Bl8OXNIKKcW3JtNG2tTvp5CGcdn6GZGCaZWldzk6J7MFZVTFAIRyRQU9JVsHd9EG09heBzto7hdDbfN9ero7r8UITPVO7i1XxfoE6k1EHShuXtPleOELjtFzm9VrzH7cn7fY" xr:uid="{90E85313-5E40-414D-9C42-229BB197B0DE}"/>
-    <hyperlink ref="C46" r:id="rId65" xr:uid="{F2BAF4A6-985D-44AC-9ECB-2096E65D0F5C}"/>
-    <hyperlink ref="D46" r:id="rId66" xr:uid="{E6F296C4-41E7-4352-9AA6-816879210698}"/>
-    <hyperlink ref="D41" r:id="rId67" xr:uid="{D0752B48-FE78-4894-B354-C5D73DF9CA15}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{FF537007-C8B6-422B-B764-A977081C356D}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{01803DF9-95A9-4673-B3CF-0AFDC51738A6}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{0A79A952-20B9-42A0-96C2-1DF0D3009FCE}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{C448F71C-0442-4884-8E94-74AB850D546C}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{CCDBF689-403E-43A8-BED9-3E755171E066}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{64183D9C-D3CF-4202-B5C3-18F54B30105D}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{63355708-FBD7-4D22-AECF-34AD1D7C138F}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{480D5B27-8454-41B3-A50B-4ACFFDAE4026}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{9FE6D3D1-53E9-489A-AB96-5EC7DADDD591}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{5D03CC0B-DEE3-4FDE-9306-CE5E26709C32}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{FFAAC713-605F-4948-894C-B32F62D6C8E4}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{0332E7E1-BC6A-47EA-89D6-97A7068AB01F}"/>
+    <hyperlink ref="C15" r:id="rId13" xr:uid="{6EC68279-7666-4082-ADEA-A2C7658064D2}"/>
+    <hyperlink ref="C16" r:id="rId14" xr:uid="{29844E65-FF0E-4D48-82B8-096506F811E6}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{28A376E3-CC6D-491B-96A1-EB17AA4EFB22}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{412FF679-225E-44C0-8E9F-CFBE4329EBC3}"/>
+    <hyperlink ref="C19" r:id="rId17" xr:uid="{7C9CB129-6FFC-4285-AC98-069E1A3CCCC6}"/>
+    <hyperlink ref="C20" r:id="rId18" xr:uid="{234F6491-E60B-4B87-A632-870076D9CCA7}"/>
+    <hyperlink ref="C21" r:id="rId19" xr:uid="{61D9836A-7C7E-4867-ABF5-33BB8C69892E}"/>
+    <hyperlink ref="C22" r:id="rId20" xr:uid="{D4605030-C409-4AF3-8259-809032BBDE3E}"/>
+    <hyperlink ref="C25" r:id="rId21" xr:uid="{080340CC-9D67-448D-91B8-CF5E61F24528}"/>
+    <hyperlink ref="C26" r:id="rId22" xr:uid="{2C13BE1F-6959-4279-B9CC-BE2550EA0D05}"/>
+    <hyperlink ref="C27" r:id="rId23" xr:uid="{161A5A2E-4114-4985-9828-82028E172B03}"/>
+    <hyperlink ref="C28" r:id="rId24" xr:uid="{11E684AC-C433-4034-B87F-E540C77A524F}"/>
+    <hyperlink ref="C29" r:id="rId25" xr:uid="{6B023398-4DAE-4F93-81D4-CF7601909568}"/>
+    <hyperlink ref="C30" r:id="rId26" xr:uid="{0C9432DA-F217-44DE-B2FF-70283A13F215}"/>
+    <hyperlink ref="C31" r:id="rId27" xr:uid="{B70145B5-B167-4A5B-8D5E-B5EBC65F3C2B}"/>
+    <hyperlink ref="C32" r:id="rId28" xr:uid="{ED6D5FE2-EE49-483E-B19B-37602DF833A2}"/>
+    <hyperlink ref="C35" r:id="rId29" xr:uid="{DBA5A372-746C-4C4C-815B-81F869194C86}"/>
+    <hyperlink ref="C36" r:id="rId30" xr:uid="{FEDE9C89-95F5-405A-B824-83ACDC1592FF}"/>
+    <hyperlink ref="C37" r:id="rId31" xr:uid="{8E39BE0E-9C8D-4504-94B0-4A6D54597337}"/>
+    <hyperlink ref="C38" r:id="rId32" xr:uid="{1ED5BD43-7A12-48C2-BC69-8F0EBCC5B3A0}"/>
+    <hyperlink ref="C39" r:id="rId33" xr:uid="{049280BA-CFC9-44A0-A076-2331B0E40C26}"/>
+    <hyperlink ref="C40" r:id="rId34" xr:uid="{9C52C1E3-7BD1-4B41-A23E-81A351F47D54}"/>
+    <hyperlink ref="C41" r:id="rId35" xr:uid="{D1BD7645-D58F-40F7-978F-383E3AB8995C}"/>
+    <hyperlink ref="C42" r:id="rId36" xr:uid="{70FE4ABE-035F-4403-A099-051396E69EF1}"/>
+    <hyperlink ref="C43" r:id="rId37" xr:uid="{A6B885F7-852B-4C3F-896A-81B7A4085B52}"/>
+    <hyperlink ref="C45" r:id="rId38" xr:uid="{7C291294-21B9-4C11-8570-25513F54FB58}"/>
+    <hyperlink ref="C44" r:id="rId39" xr:uid="{CBEA5E2B-AF57-44B8-A639-1B5A04764DA8}"/>
+    <hyperlink ref="C46" r:id="rId40" xr:uid="{F2BAF4A6-985D-44AC-9ECB-2096E65D0F5C}"/>
+    <hyperlink ref="D2" r:id="rId41" xr:uid="{29B54B0C-230F-4EBD-9F61-C5590B56DD00}"/>
+    <hyperlink ref="D3" r:id="rId42" xr:uid="{896F1657-5273-49E7-AEC6-6D2F5773145F}"/>
+    <hyperlink ref="D5" r:id="rId43" xr:uid="{7DB8FC9E-DC63-4EC9-90C8-D30329CE42AF}"/>
+    <hyperlink ref="D6" r:id="rId44" xr:uid="{A2A8BD86-402F-48A8-ACCA-5851B66D935A}"/>
+    <hyperlink ref="D9" r:id="rId45" xr:uid="{DD7E7483-3FB4-4EBE-B18F-250F1C4D853F}"/>
+    <hyperlink ref="D10" r:id="rId46" xr:uid="{82E854F4-78B0-4107-9AF8-6E66EE4AEF99}"/>
+    <hyperlink ref="D11" r:id="rId47" xr:uid="{FE647A04-AE5C-4372-8F08-5D5AA8B11DA0}"/>
+    <hyperlink ref="D13" r:id="rId48" xr:uid="{552156F6-29F8-49A4-A7F9-010D836845FF}"/>
+    <hyperlink ref="D14" r:id="rId49" xr:uid="{680ECEBD-C9B7-4796-BFA0-C7F90AD1E61C}"/>
+    <hyperlink ref="D16" r:id="rId50" xr:uid="{C243843F-1C0D-49E9-925E-219994FEE0E7}"/>
+    <hyperlink ref="D18" r:id="rId51" xr:uid="{F54E1C32-7F9D-4E11-BEEB-161F3B346EC9}"/>
+    <hyperlink ref="D19" r:id="rId52" xr:uid="{45EBB61B-4124-4F4A-9B26-B0BC95AB6804}"/>
+    <hyperlink ref="D28" r:id="rId53" xr:uid="{B9E7A496-F919-4DD5-8B97-F4D2CC837346}"/>
+    <hyperlink ref="D30" r:id="rId54" xr:uid="{EE3F23B3-0972-4AFE-AA05-C75230607DE0}"/>
+    <hyperlink ref="D31" r:id="rId55" xr:uid="{F6717058-8656-40D8-93D9-4A9CB3E42F2F}"/>
+    <hyperlink ref="D7" r:id="rId56" xr:uid="{A9F0F504-A3A0-43B3-89A9-FD2FD9781881}"/>
+    <hyperlink ref="D35" r:id="rId57" xr:uid="{14374BCA-817D-4AF8-9C27-5BBADFE600DB}"/>
+    <hyperlink ref="D37" r:id="rId58" xr:uid="{A88B7F24-726D-4822-9B5B-6358D2677EFE}"/>
+    <hyperlink ref="D38" r:id="rId59" xr:uid="{C6A70DB8-0DE1-4A9C-B684-8544DE84E6CB}"/>
+    <hyperlink ref="D40" r:id="rId60" xr:uid="{4FFDD732-8448-4687-A851-89BAFE5647B7}"/>
+    <hyperlink ref="D42" r:id="rId61" xr:uid="{A9DAB6F6-46A6-48F6-8D06-9895F4BE2DCC}"/>
+    <hyperlink ref="D45" r:id="rId62" xr:uid="{A5FECECC-616C-4D88-8071-76F20BE640A9}"/>
+    <hyperlink ref="D44" r:id="rId63" display="https://books.googleusercontent.com/books/content?req=AKW5QacMsPlzkhSCOohiXYeGljWguMgUQZpwSe9jD-AwX2dY7j4q8PfiYB4m-J-mvsYJpatZ3-Jt4fsCZCAr6gcAHgo8XQBnTUMNt41l5rsg236daxIa9HqNBkAEk1oCCB_F_p0JSetKf7xs-kEVhTq-Qbn_wXgRDnmYyENLKcPb6eOAGx0Bl8OXNIKKcW3JtNG2tTvp5CGcdn6GZGCaZWldzk6J7MFZVTFAIRyRQU9JVsHd9EG09heBzto7hdDbfN9ero7r8UITPVO7i1XxfoE6k1EHShuXtPleOELjtFzm9VrzH7cn7fY" xr:uid="{59DE3D88-69D3-4592-A0D7-73477401C393}"/>
+    <hyperlink ref="D46" r:id="rId64" xr:uid="{4451146A-BDC7-4294-B5EC-CD06DEAA48D2}"/>
+    <hyperlink ref="D41" r:id="rId65" xr:uid="{26D85D91-7304-4F95-8D61-B4C7250C1338}"/>
+    <hyperlink ref="D39" r:id="rId66" xr:uid="{072D5D06-E8E1-4CEF-A4D6-132B11F77EF8}"/>
+    <hyperlink ref="D4" r:id="rId67" xr:uid="{5EEDE8FC-2CF5-445D-9161-07E00F03BF64}"/>
+    <hyperlink ref="D8" r:id="rId68" xr:uid="{02AA18D1-3937-4FCB-B2DE-66613C65A02A}"/>
+    <hyperlink ref="D15" r:id="rId69" xr:uid="{7B4550CE-5AE5-45C1-9CD2-3F66AC3B4402}"/>
+    <hyperlink ref="D21" r:id="rId70" xr:uid="{B7BF0D8D-FD89-4981-B6FD-6619B647715A}"/>
+    <hyperlink ref="D22" r:id="rId71" xr:uid="{07B8706F-4126-48C6-A481-8BF4C59A163A}"/>
+    <hyperlink ref="D27" r:id="rId72" xr:uid="{978B10EF-2E86-4628-8F54-B0203106FDAC}"/>
+    <hyperlink ref="D34" r:id="rId73" xr:uid="{A0D1B930-2474-4105-8386-C97F9C579347}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId68"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId74"/>
 </worksheet>
 </file>
 
@@ -7425,7 +7458,7 @@
         <v>99</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>166</v>
@@ -7450,7 +7483,7 @@
         <v>337</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>294</v>
@@ -7486,7 +7519,7 @@
         <v>368</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="229.35" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
update duerer data: media id links
</commit_message>
<xml_diff>
--- a/public/data/data-duerer-macro.xlsx
+++ b/public/data/data-duerer-macro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B363D1-6217-4BEB-8442-BE7C06F1DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E296410-B24C-4770-8DA3-A587D60C4325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="2" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="539">
   <si>
     <t>id</t>
   </si>
@@ -3432,8 +3432,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3509,6 +3509,9 @@
       </c>
       <c r="B4" t="s">
         <v>295</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>296</v>
@@ -4600,7 +4603,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>

</xml_diff>